<commit_message>
draft 1 - all tasks working, data looks good. "not at all...extremely" default text removed from self reports.
</commit_message>
<xml_diff>
--- a/measures/filler_1.xlsx
+++ b/measures/filler_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/unconscious-ec-RRR/measures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D38AFF-CDB6-0A4E-977E-1A5CC1F3E162}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479B5311-6D8A-2449-B7DA-379C394CE338}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="460" windowWidth="26820" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
+    <t>filler_1_items</t>
+  </si>
+  <si>
     <t>I would prefer complex to simple problems.
 1 = strong disagreement
 2 = moderate disagreement
@@ -29,7 +32,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I like to have the responsibility of handling a situation that requires a lot of thinking.
@@ -39,7 +43,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>Thinking is not my idea of fun.
@@ -49,7 +54,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I would rather do something that requires little thought than something that is sure to challenge my thinking abilities.
@@ -59,7 +65,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I try to anticipate and avoid situations where there is likely a chance I will have to think in depth about something.
@@ -69,7 +76,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I find satisfaction in deliberating hard and for long hours.
@@ -79,7 +87,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I only think as hard as I have to.
@@ -89,7 +98,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I prefer to think about small, daily projects to long-term ones.
@@ -99,7 +109,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I like tasks that require little thought once I've learned them.
@@ -109,7 +120,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>The idea of relying on thought to make my way to the top appeals to me.
@@ -119,7 +131,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I really enjoy a task that involves coming up with new solutions to problems.
@@ -129,7 +142,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>Learning new ways to think doesn't excite me very much.
@@ -139,7 +153,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I prefer my life to be filled with puzzles that I must solve.
@@ -149,7 +164,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>The notion of thinking abstractly is appealing to me.
@@ -159,7 +175,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I would prefer a task that is intellectual, difficult, and important to one that is somewhat important but does not require much thought.
@@ -169,7 +186,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I feel relief rather than satisfaction after completing a task that required a lot of mental effort.
@@ -179,7 +197,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>It's enough for me that something gets the job done; I don't care how or why it works.
@@ -189,7 +208,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
   <si>
     <t>I usually end up deliberating about issues even when they do not affect me personally.
@@ -199,10 +219,8 @@
 4 = neither agreement nor disagreement
 5 = slight agreement
 6 = moderate agreement
-7 = strong agreement</t>
-  </si>
-  <si>
-    <t>filler_1_items</t>
+7 = strong agreement
+Click the line, then confirm your choice by clicking the grey button below.</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1087,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1079,97 +1097,97 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="184" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="183" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="204" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="204" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="204" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="207" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="297" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="230" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="170" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="170" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="170" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>